<commit_message>
update English and Japanese localization
</commit_message>
<xml_diff>
--- a/RPAStudio/RPAStudio/Localization/xStaticStrings.xlsx
+++ b/RPAStudio/RPAStudio/Localization/xStaticStrings.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SuperFly\source\repos\rpa-ai\RPAStudio\RPAStudio\RPAStudio\Localization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aww083028\source\repos\maruyama.tatsuo\RPAStudio\RPAStudio\RPAStudio\Localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC6C6A4-DB64-4E5D-A81E-E0460E839F84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4230" yWindow="3030" windowWidth="21600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4230" yWindow="3030" windowWidth="21600" windowHeight="11400"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="304">
   <si>
     <t>活动</t>
   </si>
@@ -2084,11 +2083,491 @@
     <t>AllPackagesTip</t>
     <phoneticPr fontId="3"/>
   </si>
+  <si>
+    <t>已安装</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>インストール済み</t>
+    <rPh sb="6" eb="7">
+      <t>ズ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Installed</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>InstalledText</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Uninstall</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>アンインストール</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>UninstallText</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <r>
+      <t>卸</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>载</t>
+    </r>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>VersionOnly</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>版本</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Update</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>更新</t>
+    <rPh sb="0" eb="2">
+      <t>コウシン</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>UpdateText</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>更新</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>InstallationText</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>インストール</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>安装</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Installation</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <r>
+      <t>运行</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>规则</t>
+    </r>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Operating rules</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>運用ルール</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>OperatingRule</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>すでに実行されています。多重起動はできません。</t>
+    <rPh sb="3" eb="5">
+      <t>ジッコウ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>タジュウ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>キドウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>The program is already running</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Error_AlreadyRunning</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <r>
+      <t>该</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>程序已</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>经</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>运行，不能重复运行！</t>
+    </r>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <r>
+      <t>程序运行</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>过</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>程中出</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>现</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>了异常，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>请联</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>系</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>软</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>件开</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>发</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>商！</t>
+    </r>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>An exception occurred during the program operation, please contact the software developer!</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>プログラム操作中に例外が発生しました。ソフトウェア開発者に連絡してください！</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Error_CallDeveloper</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>プログラムの実行中に重大なエラーが発生し、終了しようとしています。ソフトウェア開発者に連絡してください。</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>A serious error occurred during the running of the program, and it is about to quit. Please contact the software developer!</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Error_Critical_Exit</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <r>
+      <t>程序运行</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>过</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>程中出</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>现</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>了</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>严</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>重</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>错误</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>，即将退出，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>请联</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>系</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>软</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>件开</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>发</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>商！</t>
+    </r>
+    <phoneticPr fontId="3"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2217,7 +2696,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2231,6 +2710,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2533,11 +3015,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3500,58 +3982,130 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="3"/>
-      <c r="B69" s="3"/>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
+      <c r="A69" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="3"/>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
+      <c r="A70" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A71" s="3"/>
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
+      <c r="A71" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A72" s="3"/>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
+      <c r="A72" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A73" s="3"/>
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
+      <c r="A73" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
+      <c r="A74" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A75" s="3"/>
-      <c r="B75" s="3"/>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
+      <c r="A75" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="D75" s="10" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A76" s="3"/>
-      <c r="B76" s="3"/>
-      <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
+      <c r="A76" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A77" s="3"/>
-      <c r="B77" s="3"/>
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
+      <c r="A77" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A78" s="3"/>
@@ -3830,7 +4384,7 @@
       <c r="D123" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D68">
+  <sortState ref="A2:D68">
     <sortCondition ref="A2"/>
   </sortState>
   <phoneticPr fontId="3"/>

</xml_diff>